<commit_message>
reads in updated clear cree raw upstream passage counts from Ryan Schaefer and updates metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_upstream_passage_raw_metadata.xlsx
+++ b/data-raw/metadata/clear_upstream_passage_raw_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-clear-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB33F24C-9B21-654E-B34A-01A3E1D1EE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDF148F-AE1C-E74E-84B9-9B2638CD0E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2300" yWindow="900" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -109,13 +109,7 @@
     <t>run</t>
   </si>
   <si>
-    <t>method</t>
-  </si>
-  <si>
     <t>spawning_condition</t>
-  </si>
-  <si>
-    <t>time</t>
   </si>
   <si>
     <t>hh:mm:ss</t>
@@ -148,28 +142,13 @@
     <t>upstream_passage_raw</t>
   </si>
   <si>
-    <t>Description of spawning status based on coloration . Levels = c("full spawn coloration", NA, "unknown", "no spawn coloration",  "some spawn coloration", "post spawn")</t>
-  </si>
-  <si>
-    <t>Viewing conditions at time of data collection. Levels = c("normal", NA, "not readable", "readable")</t>
-  </si>
-  <si>
     <t>Direction of fish passage. Levels = c("up", "down")</t>
-  </si>
-  <si>
-    <t>Sex of fish observed. Levels = c("male", "unknown", "female", "not recorded")</t>
   </si>
   <si>
     <t>Date the upstream passage data were recorded</t>
   </si>
   <si>
-    <t>Time of day the upstream passage count was recorded</t>
-  </si>
-  <si>
     <t>Number of fish counted.</t>
-  </si>
-  <si>
-    <t>Assigned run of the fish viewed. Levels = c("not recorded", "spring", "unknown")</t>
   </si>
   <si>
     <t>2020-08-15</t>
@@ -178,22 +157,52 @@
     <t>2012-12-20</t>
   </si>
   <si>
-    <t>Whether or not the adipose fin was clipped. Levels = c(TRUE, FALSE, NA). Levels = c(NA, FALSE, TRUE)</t>
+    <t>time_block</t>
   </si>
   <si>
-    <t>Whether the fish is jack-sized or not. Levels = c(FALSE, NA, TRUE)</t>
+    <t>brood_year</t>
   </si>
   <si>
-    <t>Method by which the data were collected. Levels = "video"</t>
+    <t>species</t>
+  </si>
+  <si>
+    <t>time_passed</t>
+  </si>
+  <si>
+    <t>30 minute block of time out of a 24 hour day.</t>
+  </si>
+  <si>
+    <t>Brood year, defined as December 20 through August 15</t>
+  </si>
+  <si>
+    <t>Water clarity measurements at time of data collection. Levels = c("clear", "light turbidity to turbid", "flooded", "turbid to extreme turbidity")</t>
+  </si>
+  <si>
+    <t>Species of fish observed. All records for this dataset are Chinook.</t>
+  </si>
+  <si>
+    <t>The exact time the fish completely passed the white plate in the video system.</t>
+  </si>
+  <si>
+    <t>Sex of fish observed, determined by  phenotypic characteristics, kype, and tail wear. Levels = c("female", "male", "unknown", NA)</t>
+  </si>
+  <si>
+    <t>Spawning conditions (SC) measurements. c(NA, "spawning colors, defined kype, some tail wear or small amount sof fungus",  "fungus, lethargic, wandering, zombie fish; significant tail wear in females to indicate spawning in progress or has been completed",  "energetic, bright or silvery, non spawning coloration or developed secondary sex characteristics",  "energetic, can tell sex from secondary characteristics, silvery or bright coloration but may have hints of spawning colors")</t>
+  </si>
+  <si>
+    <t>Whether the fish is jack-sized or not. If a fish is under 600mm fork length, it is considered jack-size for Chinook. Levels = c(TRUE, FALSE, NA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether or not the adipose fin was clipped. Levels = c(TRUE, FALSE, NA). </t>
+  </si>
+  <si>
+    <t>Run of the fish based on spring run timing. All records are assigned spring and were observed between February 20 and August 15.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000000"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -258,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -291,7 +300,6 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="22" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,11 +515,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -590,13 +598,13 @@
         <v>20</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>16</v>
@@ -610,10 +618,10 @@
       </c>
       <c r="K2" s="14"/>
       <c r="L2" s="17" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -631,16 +639,16 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>16</v>
@@ -650,14 +658,14 @@
       <c r="H3" s="15"/>
       <c r="I3" s="14"/>
       <c r="J3" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K3" s="14"/>
       <c r="L3" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -675,38 +683,28 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>25</v>
-      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="14"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="19">
-        <v>1</v>
-      </c>
-      <c r="M4" s="15">
-        <v>1</v>
-      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -723,28 +721,38 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="F5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>25</v>
+      </c>
       <c r="I5" s="14"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19">
+        <v>1</v>
+      </c>
+      <c r="M5" s="15">
+        <v>1</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -761,16 +769,16 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>13</v>
@@ -799,16 +807,16 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>13</v>
@@ -837,16 +845,16 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>13</v>
@@ -875,28 +883,34 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>39</v>
-      </c>
       <c r="E9" s="13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="14"/>
-      <c r="J9" s="15"/>
+      <c r="J9" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="K9" s="14"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
+      <c r="L9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -913,16 +927,16 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>13</v>
@@ -951,16 +965,16 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>13</v>
@@ -989,16 +1003,16 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>13</v>
@@ -1009,8 +1023,8 @@
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
       <c r="K12" s="14"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -1025,20 +1039,68 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+    </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="A14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1093,8 +1155,8 @@
       <c r="I16" s="6"/>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1121,8 +1183,8 @@
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="5"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1205,8 +1267,8 @@
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1234,7 +1296,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="6"/>
       <c r="L21" s="11"/>
-      <c r="M21" s="5"/>
+      <c r="M21" s="11"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1289,7 +1351,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="5"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="10"/>
+      <c r="L23" s="11"/>
       <c r="M23" s="5"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1307,18 +1369,18 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="5"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1417,8 +1479,9 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
+      <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
       <c r="E28" s="1"/>
@@ -1444,9 +1507,8 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
@@ -1614,34 +1676,34 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
+      <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="1"/>
@@ -1673,29 +1735,39 @@
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
-      <c r="Z37" s="1"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="3"/>
       <c r="K38" s="2"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -1714,16 +1786,6 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="3"/>
       <c r="K39" s="2"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -1854,6 +1916,7 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
@@ -1881,7 +1944,6 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
@@ -1909,6 +1971,7 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
@@ -1936,7 +1999,6 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
@@ -2888,7 +2950,7 @@
       <c r="Z80" s="1"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1"/>
+      <c r="A81" s="4"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="2"/>
@@ -28815,18 +28877,46 @@
       <c r="Y1006" s="1"/>
       <c r="Z1006" s="1"/>
     </row>
+    <row r="1007" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="2"/>
+      <c r="E1007" s="1"/>
+      <c r="F1007" s="3"/>
+      <c r="G1007" s="3"/>
+      <c r="H1007" s="3"/>
+      <c r="I1007" s="2"/>
+      <c r="J1007" s="3"/>
+      <c r="K1007" s="2"/>
+      <c r="L1007" s="3"/>
+      <c r="M1007" s="3"/>
+      <c r="N1007" s="1"/>
+      <c r="O1007" s="1"/>
+      <c r="P1007" s="1"/>
+      <c r="Q1007" s="1"/>
+      <c r="R1007" s="1"/>
+      <c r="S1007" s="1"/>
+      <c r="T1007" s="1"/>
+      <c r="U1007" s="1"/>
+      <c r="V1007" s="1"/>
+      <c r="W1007" s="1"/>
+      <c r="X1007" s="1"/>
+      <c r="Y1007" s="1"/>
+      <c r="Z1007" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C63:C1006 C39:C51 C14:C37 C1:C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C64:C1007 C40:C52 C15:C38 C1:C14" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39:E1006 E14:E37 E1:E12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E40:E1007 E15:E38 E1:E14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F39:F1006 F14:F37 F1:F12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F40:F1007 F15:F38 F1:F14" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H39:H1006 H14:H37 H1:H12" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H40:H1007 H15:H38 H1:H14" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>